<commit_message>
PythonInExcel solution has been added.
</commit_message>
<xml_diff>
--- a/Excel Files/Excel Challenges/Challenge 270 - Case of Sentences.xlsx
+++ b/Excel Files/Excel Challenges/Challenge 270 - Case of Sentences.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\Excel-BI-Python\Excel Files\Excel Challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9CBA3F-056E-4214-9050-71668BCB2975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDFEC4AF-3E19-4B8F-A85D-D6FD2B2F1651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="34620" windowHeight="14020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,8 +57,29 @@
 </metadata>
 </file>
 
+<file path=xl/pythonScripts.xml><?xml version="1.0" encoding="utf-8"?>
+<pythonScripts xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/pythonscript">
+  <pythonScript>
+    <code>def classify_case(sentence):
+    if sentence.isupper():
+        return "All Caps"
+    elif sentence.istitle():
+        return "Start Case"
+    elif sentence.islower():
+        return "All Lowercase"
+    elif sentence[0].isupper() and sentence[1:].islower():
+        return "Sentence Case"
+    else:
+        return "Mixed Case"
+df=xl(%P2%)
+df["Case_Type"] = df[0].apply(classify_case)
+df["Case_Type"].values</code>
+  </pythonScript>
+</pythonScripts>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
   <si>
     <t>Sentence</t>
   </si>
@@ -106,6 +127,9 @@
   </si>
   <si>
     <t>Rain falls softly</t>
+  </si>
+  <si>
+    <t>Python Solution</t>
   </si>
 </sst>
 </file>
@@ -174,11 +198,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -700,6 +727,9 @@
   <we:bindings/>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
   <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{D87F86FE-615C-45B5-9D79-34F1136793EB}">
+      <we:containsCustomFunctions/>
+    </a:ext>
     <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
       <we:customFunctionIdList>
         <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
@@ -712,10 +742,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -725,9 +755,10 @@
     <col min="9" max="9" width="12.08984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.26953125" customWidth="1"/>
+    <col min="15" max="15" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -735,7 +766,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -750,8 +781,11 @@
         <f t="array" ref="M2:M10">_xlfn.LET(_xlpm.Data, A2:A10, _xlpm.IsExactMatch, _xlfn.LAMBDA(_xlpm.First,_xlpm.Second, EXACT(_xlpm.First, _xlpm.Second)), _xlpm.IsLCase, _xlpm.IsExactMatch(LOWER(_xlpm.Data), _xlpm.Data), _xlpm.IsUcase, _xlpm.IsExactMatch(UPPER(_xlpm.Data), _xlpm.Data), _xlpm.IsPCase, _xlpm.IsExactMatch(PROPER(_xlpm.Data), _xlpm.Data), _xlpm.SecondToNWardChar, MID(_xlpm.Data, 2, LEN(_xlpm.Data)), _xlpm.IsSentenceCase, _xlpm.IsExactMatch(_xlpm.Data, UPPER(LEFT(_xlpm.Data, 1)) &amp; LOWER(_xlpm.SecondToNWardChar)), _xlpm.Result, _xlfn.SWITCH(TRUE, _xlpm.IsLCase, "All Lowercase", _xlpm.IsUcase, "All Caps", _xlpm.IsPCase, "Start Case", _xlpm.IsSentenceCase, "Sentence Case", "Mixed Case"), _xlpm.Result)</f>
         <v>All Lowercase</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -764,8 +798,12 @@
       <c r="M3" t="str">
         <v>Start Case</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O3" s="4" t="str" cm="1">
+        <f t="array" ref="O3:O11">_xlfn._xlws.PY(0,0,A2:A10)</f>
+        <v>All Lowercase</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -778,8 +816,11 @@
       <c r="M4" t="str">
         <v>All Caps</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O4" t="str">
+        <v>Start Case</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -792,8 +833,11 @@
       <c r="M5" t="str">
         <v>Sentence Case</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O5" t="str">
+        <v>All Caps</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -806,8 +850,11 @@
       <c r="M6" t="str">
         <v>All Lowercase</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O6" t="str">
+        <v>Sentence Case</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -820,8 +867,11 @@
       <c r="M7" t="str">
         <v>Start Case</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O7" t="str">
+        <v>All Lowercase</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -834,8 +884,11 @@
       <c r="M8" t="str">
         <v>All Caps</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O8" t="str">
+        <v>Start Case</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -848,8 +901,11 @@
       <c r="M9" t="str">
         <v>Mixed Case</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="O9" t="str">
+        <v>All Caps</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>15</v>
       </c>
@@ -860,6 +916,14 @@
         <v>Sentence Case</v>
       </c>
       <c r="M10" t="str">
+        <v>Sentence Case</v>
+      </c>
+      <c r="O10" t="str">
+        <v>Mixed Case</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="O11" t="str">
         <v>Sentence Case</v>
       </c>
     </row>

</xml_diff>